<commit_message>
feat: fotograf haritasi guncellendi - isimli fotograflar, 2 fotografli urunler, fotografi olmayanlar bos
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/images/urun_listesi_faydalari_guncel.xlsx
+++ b/images/urun_listesi_faydalari_guncel.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cursor\Lioradg\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF1CAA6-CA0C-431F-BEE2-0897FB914AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B75F82F-B08A-4CA7-B06D-B98DD09CF95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$35</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -850,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C13:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1761,7 +1764,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>36</v>
@@ -1817,6 +1820,7 @@
       <c r="G37" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:H35" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>